<commit_message>
Running again after change in format + compute the rate_jobseek
</commit_message>
<xml_diff>
--- a/03 - Interactive Viz/amstat_nat.xlsx
+++ b/03 - Interactive Viz/amstat_nat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="3820" windowWidth="28240" windowHeight="15960"/>
+    <workbookView xWindow="5360" yWindow="3820" windowWidth="28240" windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="2.1 Taux de chômage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="80">
   <si>
     <t>Suisse alémanique</t>
   </si>
@@ -225,15 +225,6 @@
   </si>
   <si>
     <t>rate</t>
-  </si>
-  <si>
-    <t>unempl_c</t>
-  </si>
-  <si>
-    <t>jobseek_c</t>
-  </si>
-  <si>
-    <t>empl_jobseek_c</t>
   </si>
   <si>
     <t>5.2</t>
@@ -594,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -626,15 +617,6 @@
       <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
@@ -652,15 +634,9 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1">
-        <v>4911</v>
-      </c>
-      <c r="G2" s="1">
-        <v>6800</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1889</v>
-      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -678,15 +654,9 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1">
-        <v>8722</v>
-      </c>
-      <c r="G3" s="1">
-        <v>11642</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2920</v>
-      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -702,17 +672,11 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1631</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2986</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1355</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -730,15 +694,9 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
-        <v>2269</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3760</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1491</v>
-      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -756,15 +714,9 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1">
-        <v>1861</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2810</v>
-      </c>
-      <c r="H6" s="1">
-        <v>949</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -780,17 +732,11 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1653</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2491</v>
-      </c>
-      <c r="H7" s="1">
-        <v>838</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -808,15 +754,9 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1">
-        <v>1612</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2334</v>
-      </c>
-      <c r="H8" s="1">
-        <v>722</v>
-      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -834,15 +774,9 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="1">
-        <v>2539</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3309</v>
-      </c>
-      <c r="H9" s="1">
-        <v>770</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -860,15 +794,9 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1">
-        <v>4980</v>
-      </c>
-      <c r="G10" s="1">
-        <v>7323</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2343</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -886,15 +814,9 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="1">
-        <v>5739</v>
-      </c>
-      <c r="G11" s="1">
-        <v>7982</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2243</v>
-      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -912,15 +834,9 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="1">
-        <v>12546</v>
-      </c>
-      <c r="G12" s="1">
-        <v>15950</v>
-      </c>
-      <c r="H12" s="1">
-        <v>3404</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -936,17 +852,11 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="1">
-        <v>15446</v>
-      </c>
-      <c r="G13" s="1">
-        <v>19162</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3716</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -964,15 +874,9 @@
       <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="1">
-        <v>195</v>
-      </c>
-      <c r="G14" s="1">
-        <v>368</v>
-      </c>
-      <c r="H14" s="1">
-        <v>173</v>
-      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -990,15 +894,9 @@
       <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="1">
-        <v>220</v>
-      </c>
-      <c r="G15" s="1">
-        <v>337</v>
-      </c>
-      <c r="H15" s="1">
-        <v>117</v>
-      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -1016,15 +914,9 @@
       <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="1">
-        <v>621</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1154</v>
-      </c>
-      <c r="H16" s="1">
-        <v>533</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
@@ -1042,15 +934,9 @@
       <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="1">
-        <v>701</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1211</v>
-      </c>
-      <c r="H17" s="1">
-        <v>510</v>
-      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
@@ -1066,17 +952,11 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="1">
-        <v>197</v>
-      </c>
-      <c r="G18" s="1">
-        <v>334</v>
-      </c>
-      <c r="H18" s="1">
-        <v>137</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
@@ -1094,15 +974,9 @@
       <c r="E19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="1">
-        <v>346</v>
-      </c>
-      <c r="G19" s="1">
-        <v>581</v>
-      </c>
-      <c r="H19" s="1">
-        <v>235</v>
-      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
@@ -1120,15 +994,9 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="1">
-        <v>24</v>
-      </c>
-      <c r="G20" s="1">
-        <v>35</v>
-      </c>
-      <c r="H20" s="1">
-        <v>11</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
@@ -1144,17 +1012,11 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1">
-        <v>44</v>
-      </c>
-      <c r="G21" s="1">
-        <v>68</v>
-      </c>
-      <c r="H21" s="1">
-        <v>24</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -1170,17 +1032,11 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2953</v>
-      </c>
-      <c r="G22" s="1">
-        <v>5183</v>
-      </c>
-      <c r="H22" s="1">
-        <v>2230</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
@@ -1198,15 +1054,9 @@
       <c r="E23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="1">
-        <v>3101</v>
-      </c>
-      <c r="G23" s="1">
-        <v>5425</v>
-      </c>
-      <c r="H23" s="1">
-        <v>2324</v>
-      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
@@ -1224,15 +1074,9 @@
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="1">
-        <v>470</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1119</v>
-      </c>
-      <c r="H24" s="1">
-        <v>649</v>
-      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
@@ -1250,15 +1094,9 @@
       <c r="E25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="1">
-        <v>614</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1311</v>
-      </c>
-      <c r="H25" s="1">
-        <v>697</v>
-      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
@@ -1274,17 +1112,11 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1546</v>
-      </c>
-      <c r="G26" s="1">
-        <v>2814</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1268</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
@@ -1302,15 +1134,9 @@
       <c r="E27" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="1">
-        <v>1580</v>
-      </c>
-      <c r="G27" s="1">
-        <v>2875</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1295</v>
-      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
@@ -1328,15 +1154,9 @@
       <c r="E28" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="1">
-        <v>1591</v>
-      </c>
-      <c r="G28" s="1">
-        <v>2893</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1302</v>
-      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
@@ -1354,15 +1174,9 @@
       <c r="E29" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="1">
-        <v>2284</v>
-      </c>
-      <c r="G29" s="1">
-        <v>3912</v>
-      </c>
-      <c r="H29" s="1">
-        <v>1628</v>
-      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
@@ -1378,17 +1192,11 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="1">
-        <v>69</v>
-      </c>
-      <c r="G30" s="1">
-        <v>127</v>
-      </c>
-      <c r="H30" s="1">
-        <v>58</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
@@ -1406,15 +1214,9 @@
       <c r="E31" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="1">
-        <v>60</v>
-      </c>
-      <c r="G31" s="1">
-        <v>138</v>
-      </c>
-      <c r="H31" s="1">
-        <v>78</v>
-      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
@@ -1432,15 +1234,9 @@
       <c r="E32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="1">
-        <v>630</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1023</v>
-      </c>
-      <c r="H32" s="1">
-        <v>393</v>
-      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
@@ -1458,15 +1254,9 @@
       <c r="E33" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="1">
-        <v>817</v>
-      </c>
-      <c r="G33" s="1">
-        <v>1209</v>
-      </c>
-      <c r="H33" s="1">
-        <v>392</v>
-      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
@@ -1484,15 +1274,9 @@
       <c r="E34" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="1">
-        <v>79</v>
-      </c>
-      <c r="G34" s="1">
-        <v>139</v>
-      </c>
-      <c r="H34" s="1">
-        <v>60</v>
-      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
@@ -1510,15 +1294,9 @@
       <c r="E35" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="1">
-        <v>97</v>
-      </c>
-      <c r="G35" s="1">
-        <v>171</v>
-      </c>
-      <c r="H35" s="1">
-        <v>74</v>
-      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
@@ -1534,17 +1312,11 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="1">
-        <v>96</v>
-      </c>
-      <c r="G36" s="1">
-        <v>180</v>
-      </c>
-      <c r="H36" s="1">
-        <v>84</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
@@ -1562,15 +1334,9 @@
       <c r="E37" t="s">
         <v>34</v>
       </c>
-      <c r="F37" s="1">
-        <v>145</v>
-      </c>
-      <c r="G37" s="1">
-        <v>254</v>
-      </c>
-      <c r="H37" s="1">
-        <v>109</v>
-      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
@@ -1586,17 +1352,11 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="1">
-        <v>728</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1266</v>
-      </c>
-      <c r="H38" s="1">
-        <v>538</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
@@ -1614,15 +1374,9 @@
       <c r="E39" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="1">
-        <v>846</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1441</v>
-      </c>
-      <c r="H39" s="1">
-        <v>595</v>
-      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
@@ -1638,17 +1392,11 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F40" s="1">
-        <v>8143</v>
-      </c>
-      <c r="G40" s="1">
-        <v>12107</v>
-      </c>
-      <c r="H40" s="1">
-        <v>3964</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
@@ -1666,15 +1414,9 @@
       <c r="E41" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="1">
-        <v>8962</v>
-      </c>
-      <c r="G41" s="1">
-        <v>12484</v>
-      </c>
-      <c r="H41" s="1">
-        <v>3522</v>
-      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
@@ -1692,15 +1434,9 @@
       <c r="E42" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="1">
-        <v>2189</v>
-      </c>
-      <c r="G42" s="1">
-        <v>3697</v>
-      </c>
-      <c r="H42" s="1">
-        <v>1508</v>
-      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
@@ -1718,15 +1454,9 @@
       <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="1">
-        <v>2816</v>
-      </c>
-      <c r="G43" s="1">
-        <v>4302</v>
-      </c>
-      <c r="H43" s="1">
-        <v>1486</v>
-      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
@@ -1744,15 +1474,9 @@
       <c r="E44" t="s">
         <v>54</v>
       </c>
-      <c r="F44" s="1">
-        <v>5874</v>
-      </c>
-      <c r="G44" s="1">
-        <v>7686</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1812</v>
-      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
@@ -1768,17 +1492,11 @@
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="1">
-        <v>6170</v>
-      </c>
-      <c r="G45" s="1">
-        <v>7861</v>
-      </c>
-      <c r="H45" s="1">
-        <v>1691</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
@@ -1796,15 +1514,9 @@
       <c r="E46" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="1">
-        <v>1806</v>
-      </c>
-      <c r="G46" s="1">
-        <v>3422</v>
-      </c>
-      <c r="H46" s="1">
-        <v>1616</v>
-      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
@@ -1822,15 +1534,9 @@
       <c r="E47" t="s">
         <v>1</v>
       </c>
-      <c r="F47" s="1">
-        <v>2566</v>
-      </c>
-      <c r="G47" s="1">
-        <v>4333</v>
-      </c>
-      <c r="H47" s="1">
-        <v>1767</v>
-      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
@@ -1846,17 +1552,11 @@
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" s="1">
-        <v>2016</v>
-      </c>
-      <c r="G48" s="1">
-        <v>2749</v>
-      </c>
-      <c r="H48" s="1">
-        <v>733</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
@@ -1874,15 +1574,9 @@
       <c r="E49" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="1">
-        <v>2836</v>
-      </c>
-      <c r="G49" s="1">
-        <v>3756</v>
-      </c>
-      <c r="H49" s="1">
-        <v>920</v>
-      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
@@ -1898,17 +1592,11 @@
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
-      </c>
-      <c r="F50" s="1">
-        <v>535</v>
-      </c>
-      <c r="G50" s="1">
-        <v>755</v>
-      </c>
-      <c r="H50" s="1">
-        <v>220</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
@@ -1926,15 +1614,9 @@
       <c r="E51" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="1">
-        <v>1068</v>
-      </c>
-      <c r="G51" s="1">
-        <v>1659</v>
-      </c>
-      <c r="H51" s="1">
-        <v>591</v>
-      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
@@ -1950,17 +1632,11 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2206</v>
-      </c>
-      <c r="G52" s="1">
-        <v>3836</v>
-      </c>
-      <c r="H52" s="1">
-        <v>1630</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
@@ -1976,17 +1652,11 @@
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F53" s="1">
-        <v>2776</v>
-      </c>
-      <c r="G53" s="1">
-        <v>4459</v>
-      </c>
-      <c r="H53" s="1">
-        <v>1683</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="F54" s="1"/>

</xml_diff>